<commit_message>
updated formats of figs, tables, and readme
</commit_message>
<xml_diff>
--- a/SupplementalFiles/Supplemental_Table_2.xlsx
+++ b/SupplementalFiles/Supplemental_Table_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HHD/Documents/GitHub/paper-OysterSeed-TimeXTemp/SupplementalFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939A7059-8AD9-B449-AA89-8B818C606C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC9C885-5834-844A-8E5A-0F13A7DA9DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="460" windowWidth="21060" windowHeight="11020" xr2:uid="{E4D4141F-9E7A-AF49-93CF-6C29E7FAD514}"/>
   </bookViews>
@@ -79,7 +79,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Preliminary Proteome Characterization</t>
+      <t xml:space="preserve"> Preliminary proteome characterization</t>
     </r>
     <r>
       <rPr>
@@ -1685,7 +1685,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>